<commit_message>
feed4junit with excel -new
</commit_message>
<xml_diff>
--- a/testCase/testData1.xlsx
+++ b/testCase/testData1.xlsx
@@ -1,48 +1,439 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="16155" windowHeight="8505"/>
+    <workbookView windowWidth="28695" windowHeight="13050"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <t>pw</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>Enigma1</t>
+  </si>
+  <si>
+    <t>passwd1</t>
+  </si>
+  <si>
+    <t>Enigma2</t>
+  </si>
+  <si>
+    <t>passwd2</t>
+  </si>
+  <si>
+    <t>Enigma3</t>
+  </si>
+  <si>
+    <t>passwd3</t>
+  </si>
+  <si>
+    <t>Enigma4</t>
+  </si>
+  <si>
+    <t>passwd4</t>
+  </si>
+  <si>
+    <t>Enigma5</t>
+  </si>
+  <si>
+    <t>passwd5</t>
+  </si>
+  <si>
+    <t>Enigma6</t>
+  </si>
+  <si>
+    <t>passwd6</t>
+  </si>
+  <si>
+    <t>Enigma7</t>
+  </si>
+  <si>
+    <t>passwd7</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -50,9 +441,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -61,10 +694,57 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -355,50 +1035,145 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>